<commit_message>
updated with JS threats
</commit_message>
<xml_diff>
--- a/threat_risk_tables_main.xlsx
+++ b/threat_risk_tables_main.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IU\B547\B547A1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="3" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="167">
   <si>
     <t>Diagram Element</t>
   </si>
@@ -429,6 +429,141 @@
   </si>
   <si>
     <t>More advanced capabilities could overcome tamper protectioin</t>
+  </si>
+  <si>
+    <t>1.17 Invalid Password</t>
+  </si>
+  <si>
+    <t>Provide too many invalid passwords</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>1.14 User Password</t>
+  </si>
+  <si>
+    <t>Limit number of attempts before device reset</t>
+  </si>
+  <si>
+    <t>1.8 Write Valid Update</t>
+  </si>
+  <si>
+    <t>Spoof updated SW with older version which may have vulnerabilities, but is signed with an authentic key</t>
+  </si>
+  <si>
+    <t>Add list for revoked keys within device memory</t>
+  </si>
+  <si>
+    <t>1. App</t>
+  </si>
+  <si>
+    <t>Spoof the app on host computer to trick user into entering their master password</t>
+  </si>
+  <si>
+    <t>User-selected picture on startup screen</t>
+  </si>
+  <si>
+    <t>App is used on a computer with a keystroke logger</t>
+  </si>
+  <si>
+    <t>1.35 Device Reset</t>
+  </si>
+  <si>
+    <t>DoS</t>
+  </si>
+  <si>
+    <t>Perform device reset to wipe all keys</t>
+  </si>
+  <si>
+    <t>4.7 Factory Public Key</t>
+  </si>
+  <si>
+    <t>Modify device to “zero” factory public key, enabling malicious SW update</t>
+  </si>
+  <si>
+    <t>FIPS Physical Security Layer – physical intrusion</t>
+  </si>
+  <si>
+    <t>4.11 Signed User App &amp; App Public Key</t>
+  </si>
+  <si>
+    <t>Load malicious software with ability to read encrypted header and password file to enable offline password exhaustive search</t>
+  </si>
+  <si>
+    <t>Software is digitally signed using factory’s private key, and checked on USB using factory’s public key</t>
+  </si>
+  <si>
+    <t>4.18 Random Number Generator</t>
+  </si>
+  <si>
+    <t>Influence/saturate Random Number Generator during SW Update resulting in predictable pub/priv key pair</t>
+  </si>
+  <si>
+    <t>Entropy test functionality</t>
+  </si>
+  <si>
+    <t>1.34 Device Reset (Forced)</t>
+  </si>
+  <si>
+    <t>Remove power from device after it resets the counter but before it overwrites header and password file</t>
+  </si>
+  <si>
+    <t>Overwrit password file, then header file, then reset counter, in that order</t>
+  </si>
+  <si>
+    <t>1.35 Device Reset (Request)</t>
+  </si>
+  <si>
+    <t>Elevation of Privilege</t>
+  </si>
+  <si>
+    <t>Request device reset and remove power after the header file is rewritten but before the password file is rewritten to allow access to encrypted password file for offline attacks.</t>
+  </si>
+  <si>
+    <t>4.1 Message Router</t>
+  </si>
+  <si>
+    <t>Fuzz USB commands to discover readable and/or writeable device memory</t>
+  </si>
+  <si>
+    <t>Perform exhaustive read-write simulation and testing in all modes during design</t>
+  </si>
+  <si>
+    <t>Fuzz USB commands to cause unpredictable behavior and/or discover point of entry to gain execution</t>
+  </si>
+  <si>
+    <t>Perform command validation at message router, and implement a fuzz testing regime to attempt to head off most unpredictable behavior</t>
+  </si>
+  <si>
+    <t>4.30 Secure Session</t>
+  </si>
+  <si>
+    <t>Reset the device, obtain secure session with own credentials, and excavate available memory locations for old users’ password files</t>
+  </si>
+  <si>
+    <t>Perform NIST-compliant sanitization procedure during every device reset on entire password file/header memory space, prior to writing default files.</t>
+  </si>
+  <si>
+    <t>Load malicious software with ability to record shared user key during a valid user session and store in NV memory location available from secure app session for later inspection</t>
+  </si>
+  <si>
+    <t>6. Secure App Session</t>
+  </si>
+  <si>
+    <t>Hijack secure app session over USB communication, since public key is known</t>
+  </si>
+  <si>
+    <t>6. Secure User Session</t>
+  </si>
+  <si>
+    <t>Discover user key when passed during secure app session</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+  <si>
+    <t>Place reset counter in encrypted partition, write to flash vice store in memory. Do not allow decrement function. Remember previous counter state and tamper if it fails logic</t>
   </si>
 </sst>
 </file>
@@ -942,7 +1077,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -958,9 +1108,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -981,20 +1128,8 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1561,7 +1696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1575,36 +1710,36 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="54" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1613,7 +1748,7 @@
       <c r="B4" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="49" t="s">
         <v>119</v>
       </c>
       <c r="D4" s="2"/>
@@ -1628,7 +1763,7 @@
       <c r="B5" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="50" t="s">
         <v>114</v>
       </c>
       <c r="D5" s="5"/>
@@ -1643,7 +1778,7 @@
       <c r="B6" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="51" t="s">
         <v>117</v>
       </c>
       <c r="D6" s="8"/>
@@ -1658,7 +1793,7 @@
       <c r="B7" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="50" t="s">
         <v>118</v>
       </c>
       <c r="D7" s="5"/>
@@ -1670,10 +1805,10 @@
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="51" t="s">
         <v>121</v>
       </c>
       <c r="D8" s="8"/>
@@ -1686,7 +1821,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="19"/>
-      <c r="C9" s="62"/>
+      <c r="C9" s="50"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -1697,7 +1832,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="20"/>
-      <c r="C10" s="63"/>
+      <c r="C10" s="51"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -1708,7 +1843,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="19"/>
-      <c r="C11" s="62"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -1719,7 +1854,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="20"/>
-      <c r="C12" s="63"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1730,7 +1865,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="19"/>
-      <c r="C13" s="62"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -1741,7 +1876,7 @@
         <v>15</v>
       </c>
       <c r="B14" s="20"/>
-      <c r="C14" s="63"/>
+      <c r="C14" s="51"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1752,7 +1887,7 @@
         <v>16</v>
       </c>
       <c r="B15" s="19"/>
-      <c r="C15" s="62"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -1763,7 +1898,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="20"/>
-      <c r="C16" s="63"/>
+      <c r="C16" s="51"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1774,7 +1909,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="19"/>
-      <c r="C17" s="62"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -1785,7 +1920,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="20"/>
-      <c r="C18" s="63"/>
+      <c r="C18" s="51"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1796,7 +1931,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="19"/>
-      <c r="C19" s="62"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -1807,7 +1942,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="20"/>
-      <c r="C20" s="63"/>
+      <c r="C20" s="51"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1818,7 +1953,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="19"/>
-      <c r="C21" s="62"/>
+      <c r="C21" s="50"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -1829,7 +1964,7 @@
         <v>23</v>
       </c>
       <c r="B22" s="20"/>
-      <c r="C22" s="63"/>
+      <c r="C22" s="51"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -1840,7 +1975,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="19"/>
-      <c r="C23" s="62"/>
+      <c r="C23" s="50"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -1851,7 +1986,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="20"/>
-      <c r="C24" s="63"/>
+      <c r="C24" s="51"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
@@ -1862,7 +1997,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="19"/>
-      <c r="C25" s="62"/>
+      <c r="C25" s="50"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -1873,7 +2008,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="21"/>
-      <c r="C26" s="64"/>
+      <c r="C26" s="52"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
@@ -1898,20 +2033,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="6" width="49.85546875" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.5703125" style="65" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
     <col min="12" max="12" width="24.28515625" customWidth="1"/>
@@ -1919,68 +2056,72 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="49" t="s">
+      <c r="C2" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="49" t="s">
+      <c r="I2" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="49" t="s">
+      <c r="J2" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="49" t="s">
+      <c r="K2" s="54" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-    </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="55"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+    </row>
+    <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="26"/>
+      <c r="C4" s="26" t="s">
+        <v>84</v>
+      </c>
       <c r="D4" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="F4" s="26"/>
+      <c r="F4" s="48" t="s">
+        <v>166</v>
+      </c>
       <c r="G4" s="26"/>
       <c r="H4" s="26"/>
       <c r="I4" s="26"/>
@@ -2003,7 +2144,7 @@
       <c r="E5" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="31"/>
+      <c r="F5" s="47"/>
       <c r="G5" s="31"/>
       <c r="H5" s="31"/>
       <c r="I5" s="31"/>
@@ -2026,7 +2167,7 @@
       <c r="E6" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="46" t="s">
         <v>77</v>
       </c>
       <c r="G6" s="36"/>
@@ -2049,7 +2190,7 @@
         <v>78</v>
       </c>
       <c r="E7" s="47"/>
-      <c r="F7" s="31"/>
+      <c r="F7" s="47"/>
       <c r="G7" s="31"/>
       <c r="H7" s="31"/>
       <c r="I7" s="31"/>
@@ -2072,7 +2213,7 @@
       <c r="E8" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="46" t="s">
         <v>80</v>
       </c>
       <c r="G8" s="36"/>
@@ -2097,7 +2238,7 @@
       <c r="E9" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="47" t="s">
         <v>107</v>
       </c>
       <c r="G9" s="31"/>
@@ -2122,7 +2263,7 @@
       <c r="E10" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="36"/>
+      <c r="F10" s="46"/>
       <c r="G10" s="36"/>
       <c r="H10" s="36"/>
       <c r="I10" s="36"/>
@@ -2133,11 +2274,21 @@
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="31"/>
+      <c r="B11" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="F11" s="47" t="s">
+        <v>124</v>
+      </c>
       <c r="G11" s="31"/>
       <c r="H11" s="31"/>
       <c r="I11" s="31"/>
@@ -2148,41 +2299,71 @@
       <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="36"/>
+      <c r="B12" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="46" t="s">
+        <v>126</v>
+      </c>
       <c r="G12" s="36"/>
       <c r="H12" s="36"/>
       <c r="I12" s="36"/>
       <c r="J12" s="36"/>
       <c r="K12" s="37"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="31"/>
+      <c r="B13" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" s="47" t="s">
+        <v>129</v>
+      </c>
       <c r="G13" s="31"/>
       <c r="H13" s="31"/>
       <c r="I13" s="31"/>
       <c r="J13" s="31"/>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="36"/>
+      <c r="B14" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" s="46" t="s">
+        <v>132</v>
+      </c>
       <c r="G14" s="36"/>
       <c r="H14" s="36"/>
       <c r="I14" s="36"/>
@@ -2193,11 +2374,21 @@
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="31"/>
+      <c r="B15" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="F15" s="47" t="s">
+        <v>124</v>
+      </c>
       <c r="G15" s="31"/>
       <c r="H15" s="31"/>
       <c r="I15" s="31"/>
@@ -2208,232 +2399,1198 @@
       <c r="A16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="36"/>
+      <c r="B16" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="F16" s="46" t="s">
+        <v>80</v>
+      </c>
       <c r="G16" s="36"/>
       <c r="H16" s="36"/>
       <c r="I16" s="36"/>
       <c r="J16" s="36"/>
       <c r="K16" s="37"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="31"/>
+      <c r="B17" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="F17" s="47" t="s">
+        <v>139</v>
+      </c>
       <c r="G17" s="31"/>
       <c r="H17" s="31"/>
       <c r="I17" s="31"/>
       <c r="J17" s="31"/>
       <c r="K17" s="32"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="36"/>
+      <c r="B18" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="F18" s="46" t="s">
+        <v>142</v>
+      </c>
       <c r="G18" s="36"/>
       <c r="H18" s="36"/>
       <c r="I18" s="36"/>
       <c r="J18" s="36"/>
       <c r="K18" s="37"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="31"/>
+      <c r="B19" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="F19" s="47" t="s">
+        <v>145</v>
+      </c>
       <c r="G19" s="31"/>
       <c r="H19" s="31"/>
       <c r="I19" s="31"/>
       <c r="J19" s="31"/>
       <c r="K19" s="32"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="36"/>
+      <c r="B20" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="E20" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="F20" s="46" t="s">
+        <v>148</v>
+      </c>
       <c r="G20" s="36"/>
       <c r="H20" s="36"/>
       <c r="I20" s="36"/>
       <c r="J20" s="36"/>
       <c r="K20" s="37"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="31"/>
+      <c r="B21" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="F21" s="47" t="s">
+        <v>148</v>
+      </c>
       <c r="G21" s="31"/>
       <c r="H21" s="31"/>
       <c r="I21" s="31"/>
       <c r="J21" s="31"/>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="36"/>
+      <c r="B22" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="F22" s="46" t="s">
+        <v>154</v>
+      </c>
       <c r="G22" s="36"/>
       <c r="H22" s="36"/>
       <c r="I22" s="36"/>
       <c r="J22" s="36"/>
       <c r="K22" s="37"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="31"/>
+      <c r="B23" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="E23" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="F23" s="47" t="s">
+        <v>156</v>
+      </c>
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
       <c r="I23" s="31"/>
       <c r="J23" s="31"/>
       <c r="K23" s="32"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="36"/>
+      <c r="B24" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="46" t="s">
+        <v>158</v>
+      </c>
+      <c r="F24" s="46" t="s">
+        <v>159</v>
+      </c>
       <c r="G24" s="36"/>
       <c r="H24" s="36"/>
       <c r="I24" s="36"/>
       <c r="J24" s="36"/>
       <c r="K24" s="37"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="31"/>
+      <c r="B25" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C25" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="47" t="s">
+        <v>160</v>
+      </c>
+      <c r="F25" s="47" t="s">
+        <v>142</v>
+      </c>
       <c r="G25" s="31"/>
       <c r="H25" s="31"/>
       <c r="I25" s="31"/>
       <c r="J25" s="31"/>
       <c r="K25" s="32"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="43"/>
+      <c r="B26" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="F26" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="37"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="32"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="37"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="32"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+      <c r="A30" s="7"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="37"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="32"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="37"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="32"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="37"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="32"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="37"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="32"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="37"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="32"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="37"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="32"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="36"/>
+      <c r="K42" s="37"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="31"/>
+      <c r="K43" s="32"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
+      <c r="K44" s="37"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="31"/>
+      <c r="K45" s="32"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
+      <c r="K46" s="37"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
+      <c r="K47" s="32"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="36"/>
+      <c r="J48" s="36"/>
+      <c r="K48" s="37"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="31"/>
+      <c r="H49" s="31"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="31"/>
+      <c r="K49" s="32"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="7"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="36"/>
+      <c r="J50" s="36"/>
+      <c r="K50" s="37"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="47"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="31"/>
+      <c r="H51" s="31"/>
+      <c r="I51" s="31"/>
+      <c r="J51" s="31"/>
+      <c r="K51" s="32"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="36"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="46"/>
+      <c r="G52" s="36"/>
+      <c r="H52" s="36"/>
+      <c r="I52" s="36"/>
+      <c r="J52" s="36"/>
+      <c r="K52" s="37"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="47"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="31"/>
+      <c r="H53" s="31"/>
+      <c r="I53" s="31"/>
+      <c r="J53" s="31"/>
+      <c r="K53" s="32"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="7"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="36"/>
+      <c r="H54" s="36"/>
+      <c r="I54" s="36"/>
+      <c r="J54" s="36"/>
+      <c r="K54" s="37"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
+      <c r="G55" s="31"/>
+      <c r="H55" s="31"/>
+      <c r="I55" s="31"/>
+      <c r="J55" s="31"/>
+      <c r="K55" s="32"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="46"/>
+      <c r="G56" s="36"/>
+      <c r="H56" s="36"/>
+      <c r="I56" s="36"/>
+      <c r="J56" s="36"/>
+      <c r="K56" s="37"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="31"/>
+      <c r="E57" s="47"/>
+      <c r="F57" s="47"/>
+      <c r="G57" s="31"/>
+      <c r="H57" s="31"/>
+      <c r="I57" s="31"/>
+      <c r="J57" s="31"/>
+      <c r="K57" s="32"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="36"/>
+      <c r="E58" s="46"/>
+      <c r="F58" s="46"/>
+      <c r="G58" s="36"/>
+      <c r="H58" s="36"/>
+      <c r="I58" s="36"/>
+      <c r="J58" s="36"/>
+      <c r="K58" s="37"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="47"/>
+      <c r="F59" s="47"/>
+      <c r="G59" s="31"/>
+      <c r="H59" s="31"/>
+      <c r="I59" s="31"/>
+      <c r="J59" s="31"/>
+      <c r="K59" s="32"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="36"/>
+      <c r="E60" s="46"/>
+      <c r="F60" s="46"/>
+      <c r="G60" s="36"/>
+      <c r="H60" s="36"/>
+      <c r="I60" s="36"/>
+      <c r="J60" s="36"/>
+      <c r="K60" s="37"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="47"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="47"/>
+      <c r="F61" s="47"/>
+      <c r="G61" s="31"/>
+      <c r="H61" s="31"/>
+      <c r="I61" s="31"/>
+      <c r="J61" s="31"/>
+      <c r="K61" s="32"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="46"/>
+      <c r="G62" s="36"/>
+      <c r="H62" s="36"/>
+      <c r="I62" s="36"/>
+      <c r="J62" s="36"/>
+      <c r="K62" s="37"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="47"/>
+      <c r="D63" s="31"/>
+      <c r="E63" s="47"/>
+      <c r="F63" s="47"/>
+      <c r="G63" s="31"/>
+      <c r="H63" s="31"/>
+      <c r="I63" s="31"/>
+      <c r="J63" s="31"/>
+      <c r="K63" s="32"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="36"/>
+      <c r="E64" s="46"/>
+      <c r="F64" s="46"/>
+      <c r="G64" s="36"/>
+      <c r="H64" s="36"/>
+      <c r="I64" s="36"/>
+      <c r="J64" s="36"/>
+      <c r="K64" s="37"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="47"/>
+      <c r="D65" s="31"/>
+      <c r="E65" s="47"/>
+      <c r="F65" s="47"/>
+      <c r="G65" s="31"/>
+      <c r="H65" s="31"/>
+      <c r="I65" s="31"/>
+      <c r="J65" s="31"/>
+      <c r="K65" s="32"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="7"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="36"/>
+      <c r="H66" s="36"/>
+      <c r="I66" s="36"/>
+      <c r="J66" s="36"/>
+      <c r="K66" s="37"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="47"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="47"/>
+      <c r="F67" s="47"/>
+      <c r="G67" s="31"/>
+      <c r="H67" s="31"/>
+      <c r="I67" s="31"/>
+      <c r="J67" s="31"/>
+      <c r="K67" s="32"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="7"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="36"/>
+      <c r="D68" s="36"/>
+      <c r="E68" s="46"/>
+      <c r="F68" s="46"/>
+      <c r="G68" s="36"/>
+      <c r="H68" s="36"/>
+      <c r="I68" s="36"/>
+      <c r="J68" s="36"/>
+      <c r="K68" s="37"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="47"/>
+      <c r="D69" s="31"/>
+      <c r="E69" s="47"/>
+      <c r="F69" s="47"/>
+      <c r="G69" s="31"/>
+      <c r="H69" s="31"/>
+      <c r="I69" s="31"/>
+      <c r="J69" s="31"/>
+      <c r="K69" s="32"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="7"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="36"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="46"/>
+      <c r="F70" s="46"/>
+      <c r="G70" s="36"/>
+      <c r="H70" s="36"/>
+      <c r="I70" s="36"/>
+      <c r="J70" s="36"/>
+      <c r="K70" s="37"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="47"/>
+      <c r="D71" s="31"/>
+      <c r="E71" s="47"/>
+      <c r="F71" s="47"/>
+      <c r="G71" s="31"/>
+      <c r="H71" s="31"/>
+      <c r="I71" s="31"/>
+      <c r="J71" s="31"/>
+      <c r="K71" s="32"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="7"/>
+      <c r="B72" s="20"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="36"/>
+      <c r="E72" s="46"/>
+      <c r="F72" s="46"/>
+      <c r="G72" s="36"/>
+      <c r="H72" s="36"/>
+      <c r="I72" s="36"/>
+      <c r="J72" s="36"/>
+      <c r="K72" s="37"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="47"/>
+      <c r="D73" s="31"/>
+      <c r="E73" s="47"/>
+      <c r="F73" s="47"/>
+      <c r="G73" s="31"/>
+      <c r="H73" s="31"/>
+      <c r="I73" s="31"/>
+      <c r="J73" s="31"/>
+      <c r="K73" s="32"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="7"/>
+      <c r="B74" s="20"/>
+      <c r="C74" s="36"/>
+      <c r="D74" s="36"/>
+      <c r="E74" s="46"/>
+      <c r="F74" s="46"/>
+      <c r="G74" s="36"/>
+      <c r="H74" s="36"/>
+      <c r="I74" s="36"/>
+      <c r="J74" s="36"/>
+      <c r="K74" s="37"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="47"/>
+      <c r="D75" s="31"/>
+      <c r="E75" s="47"/>
+      <c r="F75" s="47"/>
+      <c r="G75" s="31"/>
+      <c r="H75" s="31"/>
+      <c r="I75" s="31"/>
+      <c r="J75" s="31"/>
+      <c r="K75" s="32"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="7"/>
+      <c r="B76" s="20"/>
+      <c r="C76" s="36"/>
+      <c r="D76" s="36"/>
+      <c r="E76" s="46"/>
+      <c r="F76" s="46"/>
+      <c r="G76" s="36"/>
+      <c r="H76" s="36"/>
+      <c r="I76" s="36"/>
+      <c r="J76" s="36"/>
+      <c r="K76" s="37"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="47"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="47"/>
+      <c r="F77" s="47"/>
+      <c r="G77" s="31"/>
+      <c r="H77" s="31"/>
+      <c r="I77" s="31"/>
+      <c r="J77" s="31"/>
+      <c r="K77" s="32"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" s="7"/>
+      <c r="B78" s="20"/>
+      <c r="C78" s="36"/>
+      <c r="D78" s="36"/>
+      <c r="E78" s="46"/>
+      <c r="F78" s="46"/>
+      <c r="G78" s="36"/>
+      <c r="H78" s="36"/>
+      <c r="I78" s="36"/>
+      <c r="J78" s="36"/>
+      <c r="K78" s="37"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="4"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="47"/>
+      <c r="D79" s="31"/>
+      <c r="E79" s="47"/>
+      <c r="F79" s="47"/>
+      <c r="G79" s="31"/>
+      <c r="H79" s="31"/>
+      <c r="I79" s="31"/>
+      <c r="J79" s="31"/>
+      <c r="K79" s="32"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="7"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="36"/>
+      <c r="D80" s="36"/>
+      <c r="E80" s="46"/>
+      <c r="F80" s="46"/>
+      <c r="G80" s="36"/>
+      <c r="H80" s="36"/>
+      <c r="I80" s="36"/>
+      <c r="J80" s="36"/>
+      <c r="K80" s="37"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="4"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="47"/>
+      <c r="D81" s="31"/>
+      <c r="E81" s="47"/>
+      <c r="F81" s="47"/>
+      <c r="G81" s="31"/>
+      <c r="H81" s="31"/>
+      <c r="I81" s="31"/>
+      <c r="J81" s="31"/>
+      <c r="K81" s="32"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" s="7"/>
+      <c r="B82" s="20"/>
+      <c r="C82" s="36"/>
+      <c r="D82" s="36"/>
+      <c r="E82" s="46"/>
+      <c r="F82" s="46"/>
+      <c r="G82" s="36"/>
+      <c r="H82" s="36"/>
+      <c r="I82" s="36"/>
+      <c r="J82" s="36"/>
+      <c r="K82" s="37"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="4"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="47"/>
+      <c r="D83" s="31"/>
+      <c r="E83" s="47"/>
+      <c r="F83" s="47"/>
+      <c r="G83" s="31"/>
+      <c r="H83" s="31"/>
+      <c r="I83" s="31"/>
+      <c r="J83" s="31"/>
+      <c r="K83" s="32"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="7"/>
+      <c r="B84" s="20"/>
+      <c r="C84" s="36"/>
+      <c r="D84" s="36"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="36"/>
+      <c r="H84" s="36"/>
+      <c r="I84" s="36"/>
+      <c r="J84" s="36"/>
+      <c r="K84" s="37"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="4"/>
+      <c r="B85" s="19"/>
+      <c r="C85" s="47"/>
+      <c r="D85" s="31"/>
+      <c r="E85" s="47"/>
+      <c r="F85" s="47"/>
+      <c r="G85" s="31"/>
+      <c r="H85" s="31"/>
+      <c r="I85" s="31"/>
+      <c r="J85" s="31"/>
+      <c r="K85" s="32"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="7"/>
+      <c r="B86" s="20"/>
+      <c r="C86" s="36"/>
+      <c r="D86" s="36"/>
+      <c r="E86" s="46"/>
+      <c r="F86" s="46"/>
+      <c r="G86" s="36"/>
+      <c r="H86" s="36"/>
+      <c r="I86" s="36"/>
+      <c r="J86" s="36"/>
+      <c r="K86" s="37"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" s="4"/>
+      <c r="B87" s="19"/>
+      <c r="C87" s="47"/>
+      <c r="D87" s="31"/>
+      <c r="E87" s="47"/>
+      <c r="F87" s="47"/>
+      <c r="G87" s="31"/>
+      <c r="H87" s="31"/>
+      <c r="I87" s="31"/>
+      <c r="J87" s="31"/>
+      <c r="K87" s="32"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="7"/>
+      <c r="B88" s="20"/>
+      <c r="C88" s="36"/>
+      <c r="D88" s="36"/>
+      <c r="E88" s="46"/>
+      <c r="F88" s="46"/>
+      <c r="G88" s="36"/>
+      <c r="H88" s="36"/>
+      <c r="I88" s="36"/>
+      <c r="J88" s="36"/>
+      <c r="K88" s="37"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" s="4"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="47"/>
+      <c r="D89" s="31"/>
+      <c r="E89" s="47"/>
+      <c r="F89" s="47"/>
+      <c r="G89" s="31"/>
+      <c r="H89" s="31"/>
+      <c r="I89" s="31"/>
+      <c r="J89" s="31"/>
+      <c r="K89" s="32"/>
+    </row>
+    <row r="90" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B90" s="20"/>
+      <c r="C90" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="D90" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="E90" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="F90" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="G90" s="36"/>
+      <c r="H90" s="36"/>
+      <c r="I90" s="36"/>
+      <c r="J90" s="36"/>
+      <c r="K90" s="37"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>163</v>
+      </c>
+      <c r="D91" t="s">
+        <v>81</v>
+      </c>
+      <c r="E91" t="s">
+        <v>164</v>
+      </c>
+      <c r="F91" s="65" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
         <v>87</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E94" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
         <v>88</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D95" t="s">
         <v>89</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E95" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
         <v>90</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D96" t="s">
         <v>91</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E96" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+    <row r="97" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
         <v>82</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D97" t="s">
         <v>92</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E97" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+    <row r="98" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
         <v>71</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D98" t="s">
         <v>93</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E98" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
+    <row r="99" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
         <v>78</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D99" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+    <row r="100" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
         <v>94</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D100" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2453,7 +3610,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A4:A26" numberStoredAsText="1"/>
+    <ignoredError sqref="A90 A4:A26" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2480,60 +3637,60 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="57"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="61"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="58"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="60"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="64"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="51" t="s">
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="49" t="s">
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="54" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
       <c r="D6" s="22" t="s">
         <v>53</v>
       </c>
@@ -2558,7 +3715,7 @@
       <c r="K6" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="L6" s="50"/>
+      <c r="L6" s="55"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -3367,60 +4524,60 @@
     </row>
     <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="55" t="s">
+      <c r="B31" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="57"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="61"/>
     </row>
     <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="58"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="59"/>
-      <c r="H32" s="59"/>
-      <c r="I32" s="59"/>
-      <c r="J32" s="60"/>
+      <c r="B32" s="62"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="64"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="49" t="s">
+      <c r="A34" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="49" t="s">
+      <c r="C34" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="51" t="s">
+      <c r="D34" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="51" t="s">
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="I34" s="52"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="49" t="s">
+      <c r="I34" s="57"/>
+      <c r="J34" s="57"/>
+      <c r="K34" s="58"/>
+      <c r="L34" s="54" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="50"/>
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
+      <c r="A35" s="55"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="55"/>
       <c r="D35" s="22" t="s">
         <v>61</v>
       </c>
@@ -3445,7 +4602,7 @@
       <c r="K35" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="L35" s="50"/>
+      <c r="L35" s="55"/>
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -4254,81 +5411,81 @@
     </row>
     <row r="60" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B61" s="55" t="s">
+      <c r="B61" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="C61" s="56"/>
-      <c r="D61" s="56"/>
-      <c r="E61" s="56"/>
-      <c r="F61" s="56"/>
-      <c r="G61" s="56"/>
-      <c r="H61" s="56"/>
-      <c r="I61" s="56"/>
-      <c r="J61" s="57"/>
+      <c r="C61" s="60"/>
+      <c r="D61" s="60"/>
+      <c r="E61" s="60"/>
+      <c r="F61" s="60"/>
+      <c r="G61" s="60"/>
+      <c r="H61" s="60"/>
+      <c r="I61" s="60"/>
+      <c r="J61" s="61"/>
     </row>
     <row r="62" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="58"/>
-      <c r="C62" s="59"/>
-      <c r="D62" s="59"/>
-      <c r="E62" s="59"/>
-      <c r="F62" s="59"/>
-      <c r="G62" s="59"/>
-      <c r="H62" s="59"/>
-      <c r="I62" s="59"/>
-      <c r="J62" s="60"/>
+      <c r="B62" s="62"/>
+      <c r="C62" s="63"/>
+      <c r="D62" s="63"/>
+      <c r="E62" s="63"/>
+      <c r="F62" s="63"/>
+      <c r="G62" s="63"/>
+      <c r="H62" s="63"/>
+      <c r="I62" s="63"/>
+      <c r="J62" s="64"/>
     </row>
     <row r="63" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="49" t="s">
+      <c r="A64" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="B64" s="49" t="s">
+      <c r="B64" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C64" s="49" t="s">
+      <c r="C64" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="D64" s="49" t="s">
+      <c r="D64" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="E64" s="49" t="s">
+      <c r="E64" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F64" s="49" t="s">
+      <c r="F64" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="G64" s="49" t="s">
+      <c r="G64" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="H64" s="49" t="s">
+      <c r="H64" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="I64" s="49" t="s">
+      <c r="I64" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="J64" s="49" t="s">
+      <c r="J64" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="K64" s="49" t="s">
+      <c r="K64" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="L64" s="49" t="s">
+      <c r="L64" s="54" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="50"/>
-      <c r="B65" s="50"/>
-      <c r="C65" s="50"/>
-      <c r="D65" s="50"/>
-      <c r="E65" s="50"/>
-      <c r="F65" s="50"/>
-      <c r="G65" s="50"/>
-      <c r="H65" s="50"/>
-      <c r="I65" s="50"/>
-      <c r="J65" s="50"/>
-      <c r="K65" s="50"/>
-      <c r="L65" s="50"/>
+      <c r="A65" s="55"/>
+      <c r="B65" s="55"/>
+      <c r="C65" s="55"/>
+      <c r="D65" s="55"/>
+      <c r="E65" s="55"/>
+      <c r="F65" s="55"/>
+      <c r="G65" s="55"/>
+      <c r="H65" s="55"/>
+      <c r="I65" s="55"/>
+      <c r="J65" s="55"/>
+      <c r="K65" s="55"/>
+      <c r="L65" s="55"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
@@ -4342,11 +5499,11 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
       <c r="I66" s="14">
-        <f>L7</f>
+        <f t="shared" ref="I66:I88" si="2">L7</f>
         <v>0</v>
       </c>
       <c r="J66" s="14">
-        <f>L36</f>
+        <f t="shared" ref="J66:J88" si="3">L36</f>
         <v>0</v>
       </c>
       <c r="K66" s="14"/>
@@ -4364,11 +5521,11 @@
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
       <c r="I67" s="15">
-        <f>L8</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J67" s="15">
-        <f>L37</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K67" s="15"/>
@@ -4386,11 +5543,11 @@
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
       <c r="I68" s="16">
-        <f>L9</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J68" s="16">
-        <f>L38</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K68" s="16"/>
@@ -4408,11 +5565,11 @@
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
       <c r="I69" s="15">
-        <f>L10</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J69" s="15">
-        <f>L39</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K69" s="15"/>
@@ -4430,11 +5587,11 @@
       <c r="G70" s="8"/>
       <c r="H70" s="8"/>
       <c r="I70" s="16">
-        <f>L11</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J70" s="16">
-        <f>L40</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K70" s="16"/>
@@ -4452,11 +5609,11 @@
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
       <c r="I71" s="15">
-        <f>L12</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J71" s="15">
-        <f>L41</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K71" s="15"/>
@@ -4474,11 +5631,11 @@
       <c r="G72" s="8"/>
       <c r="H72" s="8"/>
       <c r="I72" s="16">
-        <f>L13</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J72" s="16">
-        <f>L42</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K72" s="16"/>
@@ -4496,11 +5653,11 @@
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
       <c r="I73" s="15">
-        <f>L14</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J73" s="15">
-        <f>L43</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K73" s="15"/>
@@ -4518,11 +5675,11 @@
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
       <c r="I74" s="16">
-        <f>L15</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J74" s="16">
-        <f>L44</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K74" s="16"/>
@@ -4540,11 +5697,11 @@
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
       <c r="I75" s="15">
-        <f>L16</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J75" s="15">
-        <f>L45</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K75" s="15"/>
@@ -4562,11 +5719,11 @@
       <c r="G76" s="8"/>
       <c r="H76" s="8"/>
       <c r="I76" s="16">
-        <f>L17</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J76" s="16">
-        <f>L46</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K76" s="16"/>
@@ -4584,11 +5741,11 @@
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
       <c r="I77" s="15">
-        <f>L18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J77" s="15">
-        <f>L47</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K77" s="15"/>
@@ -4606,11 +5763,11 @@
       <c r="G78" s="8"/>
       <c r="H78" s="8"/>
       <c r="I78" s="16">
-        <f>L19</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J78" s="16">
-        <f>L48</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K78" s="16"/>
@@ -4628,11 +5785,11 @@
       <c r="G79" s="5"/>
       <c r="H79" s="5"/>
       <c r="I79" s="15">
-        <f>L20</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J79" s="15">
-        <f>L49</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K79" s="15"/>
@@ -4650,11 +5807,11 @@
       <c r="G80" s="8"/>
       <c r="H80" s="8"/>
       <c r="I80" s="16">
-        <f>L21</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J80" s="16">
-        <f>L50</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K80" s="16"/>
@@ -4672,11 +5829,11 @@
       <c r="G81" s="5"/>
       <c r="H81" s="5"/>
       <c r="I81" s="15">
-        <f>L22</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J81" s="15">
-        <f>L51</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K81" s="15"/>
@@ -4694,11 +5851,11 @@
       <c r="G82" s="8"/>
       <c r="H82" s="8"/>
       <c r="I82" s="16">
-        <f>L23</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J82" s="16">
-        <f>L52</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K82" s="16"/>
@@ -4716,11 +5873,11 @@
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
       <c r="I83" s="15">
-        <f>L24</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J83" s="15">
-        <f>L53</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K83" s="15"/>
@@ -4738,11 +5895,11 @@
       <c r="G84" s="8"/>
       <c r="H84" s="8"/>
       <c r="I84" s="16">
-        <f>L25</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J84" s="16">
-        <f>L54</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K84" s="16"/>
@@ -4760,11 +5917,11 @@
       <c r="G85" s="5"/>
       <c r="H85" s="5"/>
       <c r="I85" s="15">
-        <f>L26</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J85" s="15">
-        <f>L55</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K85" s="15"/>
@@ -4782,11 +5939,11 @@
       <c r="G86" s="8"/>
       <c r="H86" s="8"/>
       <c r="I86" s="16">
-        <f>L27</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J86" s="16">
-        <f>L56</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K86" s="16"/>
@@ -4804,11 +5961,11 @@
       <c r="G87" s="5"/>
       <c r="H87" s="5"/>
       <c r="I87" s="15">
-        <f>L28</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J87" s="15">
-        <f>L57</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K87" s="15"/>
@@ -4826,11 +5983,11 @@
       <c r="G88" s="12"/>
       <c r="H88" s="12"/>
       <c r="I88" s="17">
-        <f>L29</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J88" s="17">
-        <f>L58</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K88" s="17"/>
@@ -4838,6 +5995,23 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B2:J3"/>
+    <mergeCell ref="B61:J62"/>
+    <mergeCell ref="G64:G65"/>
+    <mergeCell ref="H64:H65"/>
+    <mergeCell ref="L64:L65"/>
+    <mergeCell ref="I64:I65"/>
+    <mergeCell ref="J64:J65"/>
+    <mergeCell ref="K64:K65"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="E64:E65"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="H5:K5"/>
@@ -4848,23 +6022,6 @@
     <mergeCell ref="H34:K34"/>
     <mergeCell ref="L34:L35"/>
     <mergeCell ref="B31:J32"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="B2:J3"/>
-    <mergeCell ref="B61:J62"/>
-    <mergeCell ref="G64:G65"/>
-    <mergeCell ref="H64:H65"/>
-    <mergeCell ref="L64:L65"/>
-    <mergeCell ref="I64:I65"/>
-    <mergeCell ref="J64:J65"/>
-    <mergeCell ref="K64:K65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4898,48 +6055,48 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="49" t="s">
+      <c r="I2" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="J2" s="49" t="s">
+      <c r="J2" s="54" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">

</xml_diff>